<commit_message>
5 - 7 trong testplan: testcase và bug report
Testcase và Bug report cho các chức năng:
- Giỏ hàng
- Đăng ký
- Đăng nhập
- Đăng xuất
</commit_message>
<xml_diff>
--- a/BugReport/BRGuest.xlsx
+++ b/BugReport/BRGuest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Tester</t>
   </si>
@@ -157,6 +157,59 @@
   </si>
   <si>
     <t>14/11/2017</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>Đăng ký tài khoản mới</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>Đăng nhập</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Đăng xuất</t>
+  </si>
+  <si>
+    <t>Đăng ký</t>
+  </si>
+  <si>
+    <t>Nhập Full name quá dài</t>
+  </si>
+  <si>
+    <t>1. Nhập Full nam: Trương Minh Phát Đạt
+2. Nhập Email Address:tmpdat1206@gmail.com
+3. Nhập Username: tmpdat
+4. Nhập Password: abc123456$
+5. Nhập lại Password: abc123456$
+6. Chọn câu hỏi: What is your favorite colors?
+7. Nhập câu trả lời: nhập 500 ký tự 'a'
+8. Tick chọn I accept terms conditions.
+9. Nhấn Register.</t>
+  </si>
+  <si>
+    <t>fatal</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng đăng ký 1 tài khoản khi nhập password quá dài</t>
+  </si>
+  <si>
+    <t>Ở trang đăng ký, nhập Fullname: Trương Minh Phát
+Đạt
+Nhập Email address: tmpdat1206@gmail.com.
+Nhập Username và ô textbox Username: tmpdat
+Nhập Password: 200 ký tự 'a'
+Nhập lại password: abc123456$
+Chọn câu hỏi: What is your favorite colors?
+Trả lời câu hỏi Security: Black
+Tick vào checkbox I accept terms conditions.
+Nhấn nút Register.</t>
   </si>
 </sst>
 </file>
@@ -166,12 +219,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -197,6 +258,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
   </fonts>
   <fills count="6">
@@ -357,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -367,64 +435,162 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFFFFFFF"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF4F81BD"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m/d/yy"/>
     </dxf>
@@ -505,95 +671,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFFFFFFF"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF4F81BD"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -634,7 +711,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:G6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:G9" totalsRowShown="0">
   <tableColumns count="7">
     <tableColumn id="1" name="No"/>
     <tableColumn id="2" name="Function ID"/>
@@ -649,15 +726,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I2" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I4" totalsRowShown="0">
   <tableColumns count="9">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Function name" dataDxfId="4"/>
-    <tableColumn id="3" name="Problem summary" dataDxfId="3"/>
-    <tableColumn id="4" name="How to reproduce it" dataDxfId="2"/>
-    <tableColumn id="10" name="Severity" dataDxfId="1"/>
+    <tableColumn id="2" name="Function name" dataDxfId="9"/>
+    <tableColumn id="3" name="Problem summary" dataDxfId="8"/>
+    <tableColumn id="4" name="How to reproduce it" dataDxfId="7"/>
+    <tableColumn id="10" name="Severity" dataDxfId="6"/>
     <tableColumn id="5" name="Reported by"/>
-    <tableColumn id="6" name="Date" dataDxfId="0"/>
+    <tableColumn id="6" name="Date" dataDxfId="5"/>
     <tableColumn id="8" name="Status"/>
     <tableColumn id="9" name="Comment"/>
   </tableColumns>
@@ -666,17 +743,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A8:A11" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A8:A11" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A8:A11"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Bug Status" dataDxfId="7"/>
+    <tableColumn id="1" name="Bug Status" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:C5" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:C5" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:C5"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Defect Severity"/>
@@ -974,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1006,7 +1083,7 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>40</v>
       </c>
       <c r="C2" s="3"/>
@@ -1049,7 +1126,7 @@
         <v>33</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1058,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1072,7 +1149,7 @@
         <v>34</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1081,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1091,7 +1168,7 @@
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>35</v>
       </c>
       <c r="D6">
@@ -1105,6 +1182,75 @@
       </c>
       <c r="G6">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1118,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1170,7 +1316,7 @@
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1179,23 +1325,76 @@
       <c r="D2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>24</v>
       </c>
       <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>40</v>
       </c>
       <c r="H2" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="3" spans="1:9" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="24">
+        <v>43072</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="199.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="24">
+        <v>43073</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1205,7 +1404,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1216,13 +1415,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1233,7 +1432,7 @@
       <c r="B2" s="5">
         <v>10</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1244,7 +1443,7 @@
       <c r="B3" s="6">
         <v>5</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1255,18 +1454,18 @@
       <c r="B4" s="7">
         <v>3</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>